<commit_message>
Small feat hackathon (#398)
## [0.72.3] - 16-04-24
### Fixed
- `ExcelImporter` was resetting `role` value to value set in rules instead of keeping value provided as arg
### Changed
- Default namespace set to `http://purl.org/cognite/neat#` instead of `http://purl.org/cognite/app#`
- OwlImporter for rules v2 has `make_compliant` set to False by default
### Added
- When creating OWL from rules, prefix will be saved under property `neat:prefix` (hence change of default namespace)
- When reading OWL if there is `neat:prefix` value will be added to `rules.metadata.prefix`
- By default we are defaulting OWL properties to min 0 and max 1 occurrence if no occurrence is set
- Added test for generation of complete rules out of partial rules
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-architect-david.xlsx
+++ b/docs/artifacts/rules/information-architect-david.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/data-modeling-lifecycle/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F67D503-315A-6040-A7B7-96C3A24A5BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAFFFDC-549F-DC48-B50B-F5A16763FF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,6 +722,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,12 +735,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="11" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8926,7 +8926,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8940,13 +8940,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -10284,16 +10284,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>

</xml_diff>